<commit_message>
reconcile internal repo with wmata-pipeline
</commit_message>
<xml_diff>
--- a/Data Preprocessing/Proportion of Households/output/walkshed_proportional_households_stations_p5.xlsx
+++ b/Data Preprocessing/Proportion of Households/output/walkshed_proportional_households_stations_p5.xlsx
@@ -472,7 +472,9 @@
       <c r="C2" t="n">
         <v>0.5289211381734656</v>
       </c>
-      <c r="D2" t="inlineStr"/>
+      <c r="D2" t="n">
+        <v>1663</v>
+      </c>
       <c r="E2" t="inlineStr">
         <is>
           <t>MSTN_062</t>
@@ -496,7 +498,9 @@
       <c r="C3" t="n">
         <v>2.075704342268258</v>
       </c>
-      <c r="D3" t="inlineStr"/>
+      <c r="D3" t="n">
+        <v>3639</v>
+      </c>
       <c r="E3" t="inlineStr">
         <is>
           <t>MSTN_001</t>
@@ -520,7 +524,9 @@
       <c r="C4" t="n">
         <v>2.214692242180993</v>
       </c>
-      <c r="D4" t="inlineStr"/>
+      <c r="D4" t="n">
+        <v>3007</v>
+      </c>
       <c r="E4" t="inlineStr">
         <is>
           <t>MSTN_002</t>
@@ -544,7 +550,9 @@
       <c r="C5" t="n">
         <v>3.184479594430494e-06</v>
       </c>
-      <c r="D5" t="inlineStr"/>
+      <c r="D5" t="n">
+        <v>1</v>
+      </c>
       <c r="E5" t="inlineStr">
         <is>
           <t>MSTN_065</t>
@@ -568,7 +576,9 @@
       <c r="C6" t="n">
         <v>0.555593559911826</v>
       </c>
-      <c r="D6" t="inlineStr"/>
+      <c r="D6" t="n">
+        <v>936</v>
+      </c>
       <c r="E6" t="inlineStr">
         <is>
           <t>MSTN_097</t>
@@ -592,7 +602,9 @@
       <c r="C7" t="n">
         <v>11.60390689361429</v>
       </c>
-      <c r="D7" t="inlineStr"/>
+      <c r="D7" t="n">
+        <v>13574</v>
+      </c>
       <c r="E7" t="inlineStr">
         <is>
           <t>MSTN_068</t>
@@ -616,7 +628,9 @@
       <c r="C8" t="n">
         <v>3.30480552984339</v>
       </c>
-      <c r="D8" t="inlineStr"/>
+      <c r="D8" t="n">
+        <v>4621</v>
+      </c>
       <c r="E8" t="inlineStr">
         <is>
           <t>MSTN_003</t>
@@ -640,7 +654,9 @@
       <c r="C9" t="n">
         <v>5.234589199011619</v>
       </c>
-      <c r="D9" t="inlineStr"/>
+      <c r="D9" t="n">
+        <v>7416</v>
+      </c>
       <c r="E9" t="inlineStr">
         <is>
           <t>MSTN_052</t>
@@ -664,7 +680,9 @@
       <c r="C10" t="n">
         <v>4.151525936373063</v>
       </c>
-      <c r="D10" t="inlineStr"/>
+      <c r="D10" t="n">
+        <v>5447</v>
+      </c>
       <c r="E10" t="inlineStr">
         <is>
           <t>MSTN_078</t>
@@ -688,7 +706,9 @@
       <c r="C11" t="n">
         <v>1.739792426464603</v>
       </c>
-      <c r="D11" t="inlineStr"/>
+      <c r="D11" t="n">
+        <v>2494</v>
+      </c>
       <c r="E11" t="inlineStr">
         <is>
           <t>MSTN_077</t>
@@ -712,7 +732,9 @@
       <c r="C12" t="n">
         <v>1.958217042073654</v>
       </c>
-      <c r="D12" t="inlineStr"/>
+      <c r="D12" t="n">
+        <v>3009</v>
+      </c>
       <c r="E12" t="inlineStr">
         <is>
           <t>MSTN_004</t>
@@ -736,7 +758,9 @@
       <c r="C13" t="n">
         <v>1.811875284942231</v>
       </c>
-      <c r="D13" t="inlineStr"/>
+      <c r="D13" t="n">
+        <v>2576</v>
+      </c>
       <c r="E13" t="inlineStr">
         <is>
           <t>MSTN_084</t>
@@ -760,7 +784,9 @@
       <c r="C14" t="n">
         <v>4.035045741777153</v>
       </c>
-      <c r="D14" t="inlineStr"/>
+      <c r="D14" t="n">
+        <v>6357</v>
+      </c>
       <c r="E14" t="inlineStr">
         <is>
           <t>MSTN_005</t>
@@ -784,7 +810,9 @@
       <c r="C15" t="n">
         <v>0.1759818391374898</v>
       </c>
-      <c r="D15" t="inlineStr"/>
+      <c r="D15" t="n">
+        <v>428</v>
+      </c>
       <c r="E15" t="inlineStr">
         <is>
           <t>MSTN_058</t>
@@ -808,7 +836,9 @@
       <c r="C16" t="n">
         <v>6.035049087272787</v>
       </c>
-      <c r="D16" t="inlineStr"/>
+      <c r="D16" t="n">
+        <v>8274</v>
+      </c>
       <c r="E16" t="inlineStr">
         <is>
           <t>MSTN_063</t>
@@ -832,7 +862,9 @@
       <c r="C17" t="n">
         <v>4.76463883419382</v>
       </c>
-      <c r="D17" t="inlineStr"/>
+      <c r="D17" t="n">
+        <v>6140</v>
+      </c>
       <c r="E17" t="inlineStr">
         <is>
           <t>MSTN_006</t>
@@ -856,7 +888,9 @@
       <c r="C18" t="n">
         <v>0.6358575517057929</v>
       </c>
-      <c r="D18" t="inlineStr"/>
+      <c r="D18" t="n">
+        <v>863</v>
+      </c>
       <c r="E18" t="inlineStr">
         <is>
           <t>MSTN_053</t>
@@ -880,7 +914,9 @@
       <c r="C19" t="n">
         <v>13.76915509052395</v>
       </c>
-      <c r="D19" t="inlineStr"/>
+      <c r="D19" t="n">
+        <v>18900</v>
+      </c>
       <c r="E19" t="inlineStr">
         <is>
           <t>MSTN_007</t>
@@ -904,7 +940,9 @@
       <c r="C20" t="n">
         <v>2.054893578947575</v>
       </c>
-      <c r="D20" t="inlineStr"/>
+      <c r="D20" t="n">
+        <v>3388</v>
+      </c>
       <c r="E20" t="inlineStr">
         <is>
           <t>MSTN_008</t>
@@ -928,7 +966,9 @@
       <c r="C21" t="n">
         <v>10.88604067144139</v>
       </c>
-      <c r="D21" t="inlineStr"/>
+      <c r="D21" t="n">
+        <v>14055</v>
+      </c>
       <c r="E21" t="inlineStr">
         <is>
           <t>MSTN_061</t>
@@ -952,7 +992,9 @@
       <c r="C22" t="n">
         <v>6.977318518851717</v>
       </c>
-      <c r="D22" t="inlineStr"/>
+      <c r="D22" t="n">
+        <v>10422</v>
+      </c>
       <c r="E22" t="inlineStr">
         <is>
           <t>MSTN_072</t>
@@ -976,7 +1018,9 @@
       <c r="C23" t="n">
         <v>1.625292537893846</v>
       </c>
-      <c r="D23" t="inlineStr"/>
+      <c r="D23" t="n">
+        <v>1950</v>
+      </c>
       <c r="E23" t="inlineStr">
         <is>
           <t>MSTN_009</t>
@@ -1000,7 +1044,9 @@
       <c r="C24" t="n">
         <v>3.449160006366248</v>
       </c>
-      <c r="D24" t="inlineStr"/>
+      <c r="D24" t="n">
+        <v>4284</v>
+      </c>
       <c r="E24" t="inlineStr">
         <is>
           <t>MSTN_067</t>
@@ -1024,7 +1070,9 @@
       <c r="C25" t="n">
         <v>13.99721203294711</v>
       </c>
-      <c r="D25" t="inlineStr"/>
+      <c r="D25" t="n">
+        <v>17941</v>
+      </c>
       <c r="E25" t="inlineStr">
         <is>
           <t>MSTN_010</t>
@@ -1048,7 +1096,9 @@
       <c r="C26" t="n">
         <v>1.232589060735501</v>
       </c>
-      <c r="D26" t="inlineStr"/>
+      <c r="D26" t="n">
+        <v>2136</v>
+      </c>
       <c r="E26" t="inlineStr">
         <is>
           <t>MSTN_064</t>
@@ -1072,7 +1122,9 @@
       <c r="C27" t="n">
         <v>6.203669617308431</v>
       </c>
-      <c r="D27" t="inlineStr"/>
+      <c r="D27" t="n">
+        <v>8133</v>
+      </c>
       <c r="E27" t="inlineStr">
         <is>
           <t>MSTN_011</t>
@@ -1096,7 +1148,9 @@
       <c r="C28" t="n">
         <v>1.826128817087749</v>
       </c>
-      <c r="D28" t="inlineStr"/>
+      <c r="D28" t="n">
+        <v>3227</v>
+      </c>
       <c r="E28" t="inlineStr">
         <is>
           <t>MSTN_080</t>
@@ -1120,7 +1174,9 @@
       <c r="C29" t="n">
         <v>4.159171564132368</v>
       </c>
-      <c r="D29" t="inlineStr"/>
+      <c r="D29" t="n">
+        <v>7579</v>
+      </c>
       <c r="E29" t="inlineStr">
         <is>
           <t>MSTN_012</t>
@@ -1144,7 +1200,9 @@
       <c r="C30" t="n">
         <v>2.023713651158346</v>
       </c>
-      <c r="D30" t="inlineStr"/>
+      <c r="D30" t="n">
+        <v>5307</v>
+      </c>
       <c r="E30" t="inlineStr">
         <is>
           <t>MSTN_013</t>
@@ -1168,7 +1226,9 @@
       <c r="C31" t="n">
         <v>1.900902407018739</v>
       </c>
-      <c r="D31" t="inlineStr"/>
+      <c r="D31" t="n">
+        <v>4308</v>
+      </c>
       <c r="E31" t="inlineStr">
         <is>
           <t>MSTN_014</t>
@@ -1192,7 +1252,9 @@
       <c r="C32" t="n">
         <v>0.9221150821487412</v>
       </c>
-      <c r="D32" t="inlineStr"/>
+      <c r="D32" t="n">
+        <v>1523</v>
+      </c>
       <c r="E32" t="inlineStr">
         <is>
           <t>MSTN_015</t>
@@ -1216,7 +1278,9 @@
       <c r="C33" t="n">
         <v>9.744759918765665</v>
       </c>
-      <c r="D33" t="inlineStr"/>
+      <c r="D33" t="n">
+        <v>11192</v>
+      </c>
       <c r="E33" t="inlineStr">
         <is>
           <t>MSTN_016</t>
@@ -1240,7 +1304,9 @@
       <c r="C34" t="n">
         <v>1.453957236418227</v>
       </c>
-      <c r="D34" t="inlineStr"/>
+      <c r="D34" t="n">
+        <v>2472</v>
+      </c>
       <c r="E34" t="inlineStr">
         <is>
           <t>MSTN_048</t>
@@ -1264,7 +1330,9 @@
       <c r="C35" t="n">
         <v>1.919440889686358</v>
       </c>
-      <c r="D35" t="inlineStr"/>
+      <c r="D35" t="n">
+        <v>3848</v>
+      </c>
       <c r="E35" t="inlineStr">
         <is>
           <t>MSTN_017</t>
@@ -1288,7 +1356,9 @@
       <c r="C36" t="n">
         <v>0.8969834923268065</v>
       </c>
-      <c r="D36" t="inlineStr"/>
+      <c r="D36" t="n">
+        <v>2503</v>
+      </c>
       <c r="E36" t="inlineStr">
         <is>
           <t>MSTN_083</t>
@@ -1312,7 +1382,9 @@
       <c r="C37" t="n">
         <v>5.474632801939199</v>
       </c>
-      <c r="D37" t="inlineStr"/>
+      <c r="D37" t="n">
+        <v>6978</v>
+      </c>
       <c r="E37" t="inlineStr">
         <is>
           <t>MSTN_018</t>
@@ -1336,7 +1408,9 @@
       <c r="C38" t="n">
         <v>8.994292611995219</v>
       </c>
-      <c r="D38" t="inlineStr"/>
+      <c r="D38" t="n">
+        <v>11359</v>
+      </c>
       <c r="E38" t="inlineStr">
         <is>
           <t>MSTN_019</t>
@@ -1360,7 +1434,9 @@
       <c r="C39" t="n">
         <v>7.083212115936227</v>
       </c>
-      <c r="D39" t="inlineStr"/>
+      <c r="D39" t="n">
+        <v>9826</v>
+      </c>
       <c r="E39" t="inlineStr">
         <is>
           <t>MSTN_020</t>
@@ -1384,7 +1460,9 @@
       <c r="C40" t="n">
         <v>1.46812151205189</v>
       </c>
-      <c r="D40" t="inlineStr"/>
+      <c r="D40" t="n">
+        <v>2784</v>
+      </c>
       <c r="E40" t="inlineStr">
         <is>
           <t>MSTN_044</t>
@@ -1408,7 +1486,9 @@
       <c r="C41" t="n">
         <v>0.5101893128769286</v>
       </c>
-      <c r="D41" t="inlineStr"/>
+      <c r="D41" t="n">
+        <v>1246</v>
+      </c>
       <c r="E41" t="inlineStr">
         <is>
           <t>MSTN_049</t>
@@ -1432,7 +1512,9 @@
       <c r="C42" t="n">
         <v>1.111353740023231</v>
       </c>
-      <c r="D42" t="inlineStr"/>
+      <c r="D42" t="n">
+        <v>3910</v>
+      </c>
       <c r="E42" t="inlineStr">
         <is>
           <t>MSTN_089</t>
@@ -1456,7 +1538,9 @@
       <c r="C43" t="n">
         <v>3.937019095096048</v>
       </c>
-      <c r="D43" t="inlineStr"/>
+      <c r="D43" t="n">
+        <v>5813</v>
+      </c>
       <c r="E43" t="inlineStr">
         <is>
           <t>MSTN_047</t>
@@ -1480,7 +1564,9 @@
       <c r="C44" t="n">
         <v>3.162757358875165</v>
       </c>
-      <c r="D44" t="inlineStr"/>
+      <c r="D44" t="n">
+        <v>5179</v>
+      </c>
       <c r="E44" t="inlineStr">
         <is>
           <t>MSTN_082</t>
@@ -1504,7 +1590,9 @@
       <c r="C45" t="n">
         <v>0.2529041850762535</v>
       </c>
-      <c r="D45" t="inlineStr"/>
+      <c r="D45" t="n">
+        <v>1963</v>
+      </c>
       <c r="E45" t="inlineStr">
         <is>
           <t>MSTN_093</t>
@@ -1528,7 +1616,9 @@
       <c r="C46" t="n">
         <v>1.776835234146163</v>
       </c>
-      <c r="D46" t="inlineStr"/>
+      <c r="D46" t="n">
+        <v>3053</v>
+      </c>
       <c r="E46" t="inlineStr">
         <is>
           <t>MSTN_094</t>
@@ -1552,7 +1642,9 @@
       <c r="C47" t="n">
         <v>6.579155890501085</v>
       </c>
-      <c r="D47" t="inlineStr"/>
+      <c r="D47" t="n">
+        <v>7602</v>
+      </c>
       <c r="E47" t="inlineStr">
         <is>
           <t>MSTN_021</t>
@@ -1576,7 +1668,9 @@
       <c r="C48" t="n">
         <v>3.912976092768805</v>
       </c>
-      <c r="D48" t="inlineStr"/>
+      <c r="D48" t="n">
+        <v>5552</v>
+      </c>
       <c r="E48" t="inlineStr">
         <is>
           <t>MSTN_079</t>
@@ -1600,7 +1694,9 @@
       <c r="C49" t="n">
         <v>2.066710080066629</v>
       </c>
-      <c r="D49" t="inlineStr"/>
+      <c r="D49" t="n">
+        <v>4148</v>
+      </c>
       <c r="E49" t="inlineStr">
         <is>
           <t>MSTN_022</t>
@@ -1624,7 +1720,9 @@
       <c r="C50" t="n">
         <v>0.06338833887076503</v>
       </c>
-      <c r="D50" t="inlineStr"/>
+      <c r="D50" t="n">
+        <v>775</v>
+      </c>
       <c r="E50" t="inlineStr">
         <is>
           <t>MSTN_057</t>
@@ -1648,7 +1746,9 @@
       <c r="C51" t="n">
         <v>1.066802009105359</v>
       </c>
-      <c r="D51" t="inlineStr"/>
+      <c r="D51" t="n">
+        <v>1947</v>
+      </c>
       <c r="E51" t="inlineStr">
         <is>
           <t>MSTN_085</t>
@@ -1672,7 +1772,9 @@
       <c r="C52" t="n">
         <v>0</v>
       </c>
-      <c r="D52" t="inlineStr"/>
+      <c r="D52" t="n">
+        <v>0</v>
+      </c>
       <c r="E52" t="inlineStr">
         <is>
           <t>MSTN_096</t>
@@ -1696,7 +1798,9 @@
       <c r="C53" t="n">
         <v>1.341390492554759</v>
       </c>
-      <c r="D53" t="inlineStr"/>
+      <c r="D53" t="n">
+        <v>2442</v>
+      </c>
       <c r="E53" t="inlineStr">
         <is>
           <t>MSTN_087</t>
@@ -1720,7 +1824,9 @@
       <c r="C54" t="n">
         <v>5.946756656256284</v>
       </c>
-      <c r="D54" t="inlineStr"/>
+      <c r="D54" t="n">
+        <v>8897</v>
+      </c>
       <c r="E54" t="inlineStr">
         <is>
           <t>MSTN_023</t>
@@ -1744,7 +1850,9 @@
       <c r="C55" t="n">
         <v>1.061846862282695</v>
       </c>
-      <c r="D55" t="inlineStr"/>
+      <c r="D55" t="n">
+        <v>2620</v>
+      </c>
       <c r="E55" t="inlineStr">
         <is>
           <t>MSTN_050</t>
@@ -1768,7 +1876,9 @@
       <c r="C56" t="n">
         <v>4.876675909612477</v>
       </c>
-      <c r="D56" t="inlineStr"/>
+      <c r="D56" t="n">
+        <v>7119</v>
+      </c>
       <c r="E56" t="inlineStr">
         <is>
           <t>MSTN_024</t>
@@ -1792,7 +1902,9 @@
       <c r="C57" t="n">
         <v>2.831887578400319</v>
       </c>
-      <c r="D57" t="inlineStr"/>
+      <c r="D57" t="n">
+        <v>4181</v>
+      </c>
       <c r="E57" t="inlineStr">
         <is>
           <t>MSTN_025</t>
@@ -1816,7 +1928,9 @@
       <c r="C58" t="n">
         <v>0.8822057255392796</v>
       </c>
-      <c r="D58" t="inlineStr"/>
+      <c r="D58" t="n">
+        <v>1920</v>
+      </c>
       <c r="E58" t="inlineStr">
         <is>
           <t>MSTN_086</t>
@@ -1840,7 +1954,9 @@
       <c r="C59" t="n">
         <v>14.02563379947269</v>
       </c>
-      <c r="D59" t="inlineStr"/>
+      <c r="D59" t="n">
+        <v>17532</v>
+      </c>
       <c r="E59" t="inlineStr">
         <is>
           <t>MSTN_026</t>
@@ -1864,7 +1980,9 @@
       <c r="C60" t="n">
         <v>10.40488401171169</v>
       </c>
-      <c r="D60" t="inlineStr"/>
+      <c r="D60" t="n">
+        <v>13817</v>
+      </c>
       <c r="E60" t="inlineStr">
         <is>
           <t>MSTN_027</t>
@@ -1888,7 +2006,9 @@
       <c r="C61" t="n">
         <v>1.267880790337268</v>
       </c>
-      <c r="D61" t="inlineStr"/>
+      <c r="D61" t="n">
+        <v>3387</v>
+      </c>
       <c r="E61" t="inlineStr">
         <is>
           <t>MSTN_074</t>
@@ -1912,7 +2032,9 @@
       <c r="C62" t="n">
         <v>0.584133646628592</v>
       </c>
-      <c r="D62" t="inlineStr"/>
+      <c r="D62" t="n">
+        <v>1279</v>
+      </c>
       <c r="E62" t="inlineStr">
         <is>
           <t>MSTN_056</t>
@@ -1936,7 +2058,9 @@
       <c r="C63" t="n">
         <v>10.18923317062292</v>
       </c>
-      <c r="D63" t="inlineStr"/>
+      <c r="D63" t="n">
+        <v>11738</v>
+      </c>
       <c r="E63" t="inlineStr">
         <is>
           <t>MSTN_028</t>
@@ -1960,7 +2084,9 @@
       <c r="C64" t="n">
         <v>0.07252312793337068</v>
       </c>
-      <c r="D64" t="inlineStr"/>
+      <c r="D64" t="n">
+        <v>1460</v>
+      </c>
       <c r="E64" t="inlineStr">
         <is>
           <t>MSTN_070</t>
@@ -1984,7 +2110,9 @@
       <c r="C65" t="n">
         <v>8.620887013880086</v>
       </c>
-      <c r="D65" t="inlineStr"/>
+      <c r="D65" t="n">
+        <v>11844</v>
+      </c>
       <c r="E65" t="inlineStr">
         <is>
           <t>MSTN_071</t>
@@ -2008,7 +2136,9 @@
       <c r="C66" t="n">
         <v>4.891566119623562</v>
       </c>
-      <c r="D66" t="inlineStr"/>
+      <c r="D66" t="n">
+        <v>5571</v>
+      </c>
       <c r="E66" t="inlineStr">
         <is>
           <t>MSTN_029</t>
@@ -2032,7 +2162,9 @@
       <c r="C67" t="n">
         <v>2.045581814658333</v>
       </c>
-      <c r="D67" t="inlineStr"/>
+      <c r="D67" t="n">
+        <v>4896</v>
+      </c>
       <c r="E67" t="inlineStr">
         <is>
           <t>MSTN_054</t>
@@ -2056,7 +2188,9 @@
       <c r="C68" t="n">
         <v>2.392112685101351</v>
       </c>
-      <c r="D68" t="inlineStr"/>
+      <c r="D68" t="n">
+        <v>4156</v>
+      </c>
       <c r="E68" t="inlineStr">
         <is>
           <t>MSTN_030</t>
@@ -2080,7 +2214,9 @@
       <c r="C69" t="n">
         <v>2.638527250097382</v>
       </c>
-      <c r="D69" t="inlineStr"/>
+      <c r="D69" t="n">
+        <v>4014</v>
+      </c>
       <c r="E69" t="inlineStr">
         <is>
           <t>MSTN_042</t>
@@ -2104,7 +2240,9 @@
       <c r="C70" t="n">
         <v>0.008392496060353423</v>
       </c>
-      <c r="D70" t="inlineStr"/>
+      <c r="D70" t="n">
+        <v>814</v>
+      </c>
       <c r="E70" t="inlineStr">
         <is>
           <t>MSTN_073</t>
@@ -2128,7 +2266,9 @@
       <c r="C71" t="n">
         <v>6.706443499624397</v>
       </c>
-      <c r="D71" t="inlineStr"/>
+      <c r="D71" t="n">
+        <v>8579</v>
+      </c>
       <c r="E71" t="inlineStr">
         <is>
           <t>MSTN_060</t>
@@ -2152,7 +2292,9 @@
       <c r="C72" t="n">
         <v>0.983247545888329</v>
       </c>
-      <c r="D72" t="inlineStr"/>
+      <c r="D72" t="n">
+        <v>2699</v>
+      </c>
       <c r="E72" t="inlineStr">
         <is>
           <t>MSTN_092</t>
@@ -2176,7 +2318,9 @@
       <c r="C73" t="n">
         <v>1.550426879372979</v>
       </c>
-      <c r="D73" t="inlineStr"/>
+      <c r="D73" t="n">
+        <v>3319</v>
+      </c>
       <c r="E73" t="inlineStr">
         <is>
           <t>MSTN_041</t>
@@ -2200,7 +2344,9 @@
       <c r="C74" t="n">
         <v>10.20776735321576</v>
       </c>
-      <c r="D74" t="inlineStr"/>
+      <c r="D74" t="n">
+        <v>13014</v>
+      </c>
       <c r="E74" t="inlineStr">
         <is>
           <t>MSTN_031</t>
@@ -2224,7 +2370,9 @@
       <c r="C75" t="n">
         <v>10.98315568001667</v>
       </c>
-      <c r="D75" t="inlineStr"/>
+      <c r="D75" t="n">
+        <v>13495</v>
+      </c>
       <c r="E75" t="inlineStr">
         <is>
           <t>MSTN_051</t>
@@ -2248,7 +2396,9 @@
       <c r="C76" t="n">
         <v>0.4832542598474346</v>
       </c>
-      <c r="D76" t="inlineStr"/>
+      <c r="D76" t="n">
+        <v>1344</v>
+      </c>
       <c r="E76" t="inlineStr">
         <is>
           <t>MSTN_032</t>
@@ -2272,7 +2422,9 @@
       <c r="C77" t="n">
         <v>0.377302363909378</v>
       </c>
-      <c r="D77" t="inlineStr"/>
+      <c r="D77" t="n">
+        <v>1564</v>
+      </c>
       <c r="E77" t="inlineStr">
         <is>
           <t>MSTN_076</t>
@@ -2296,7 +2448,9 @@
       <c r="C78" t="n">
         <v>1.415940941344668</v>
       </c>
-      <c r="D78" t="inlineStr"/>
+      <c r="D78" t="n">
+        <v>3362</v>
+      </c>
       <c r="E78" t="inlineStr">
         <is>
           <t>MSTN_090</t>
@@ -2320,7 +2474,9 @@
       <c r="C79" t="n">
         <v>2.802979900222979</v>
       </c>
-      <c r="D79" t="inlineStr"/>
+      <c r="D79" t="n">
+        <v>3763</v>
+      </c>
       <c r="E79" t="inlineStr">
         <is>
           <t>MSTN_033</t>
@@ -2344,7 +2500,9 @@
       <c r="C80" t="n">
         <v>0.8388715032951091</v>
       </c>
-      <c r="D80" t="inlineStr"/>
+      <c r="D80" t="n">
+        <v>2723</v>
+      </c>
       <c r="E80" t="inlineStr">
         <is>
           <t>MSTN_075</t>
@@ -2368,7 +2526,9 @@
       <c r="C81" t="n">
         <v>2.392571914347609</v>
       </c>
-      <c r="D81" t="inlineStr"/>
+      <c r="D81" t="n">
+        <v>3477</v>
+      </c>
       <c r="E81" t="inlineStr">
         <is>
           <t>MSTN_034</t>
@@ -2392,7 +2552,9 @@
       <c r="C82" t="n">
         <v>2.25631443108501</v>
       </c>
-      <c r="D82" t="inlineStr"/>
+      <c r="D82" t="n">
+        <v>3973</v>
+      </c>
       <c r="E82" t="inlineStr">
         <is>
           <t>MSTN_035</t>
@@ -2416,7 +2578,9 @@
       <c r="C83" t="n">
         <v>2.588010033338184</v>
       </c>
-      <c r="D83" t="inlineStr"/>
+      <c r="D83" t="n">
+        <v>4559</v>
+      </c>
       <c r="E83" t="inlineStr">
         <is>
           <t>MSTN_043</t>
@@ -2440,7 +2604,9 @@
       <c r="C84" t="n">
         <v>0.6451965388329074</v>
       </c>
-      <c r="D84" t="inlineStr"/>
+      <c r="D84" t="n">
+        <v>1056</v>
+      </c>
       <c r="E84" t="inlineStr">
         <is>
           <t>MSTN_088</t>
@@ -2464,7 +2630,9 @@
       <c r="C85" t="n">
         <v>13.22060104232712</v>
       </c>
-      <c r="D85" t="inlineStr"/>
+      <c r="D85" t="n">
+        <v>16909</v>
+      </c>
       <c r="E85" t="inlineStr">
         <is>
           <t>MSTN_036</t>
@@ -2488,7 +2656,9 @@
       <c r="C86" t="n">
         <v>3.200288033636398</v>
       </c>
-      <c r="D86" t="inlineStr"/>
+      <c r="D86" t="n">
+        <v>5769</v>
+      </c>
       <c r="E86" t="inlineStr">
         <is>
           <t>MSTN_037</t>
@@ -2512,7 +2682,9 @@
       <c r="C87" t="n">
         <v>0.3466421120293831</v>
       </c>
-      <c r="D87" t="inlineStr"/>
+      <c r="D87" t="n">
+        <v>1750</v>
+      </c>
       <c r="E87" t="inlineStr">
         <is>
           <t>MSTN_081</t>
@@ -2536,7 +2708,9 @@
       <c r="C88" t="n">
         <v>5.139097327930192</v>
       </c>
-      <c r="D88" t="inlineStr"/>
+      <c r="D88" t="n">
+        <v>6915</v>
+      </c>
       <c r="E88" t="inlineStr">
         <is>
           <t>MSTN_038</t>
@@ -2560,7 +2734,9 @@
       <c r="C89" t="n">
         <v>2.592498324463673</v>
       </c>
-      <c r="D89" t="inlineStr"/>
+      <c r="D89" t="n">
+        <v>3767</v>
+      </c>
       <c r="E89" t="inlineStr">
         <is>
           <t>MSTN_069</t>
@@ -2584,7 +2760,9 @@
       <c r="C90" t="n">
         <v>8.773784606229452</v>
       </c>
-      <c r="D90" t="inlineStr"/>
+      <c r="D90" t="n">
+        <v>10940</v>
+      </c>
       <c r="E90" t="inlineStr">
         <is>
           <t>MSTN_066</t>
@@ -2608,7 +2786,9 @@
       <c r="C91" t="n">
         <v>9.337732267289686</v>
       </c>
-      <c r="D91" t="inlineStr"/>
+      <c r="D91" t="n">
+        <v>11179</v>
+      </c>
       <c r="E91" t="inlineStr">
         <is>
           <t>MSTN_039</t>
@@ -2632,7 +2812,9 @@
       <c r="C92" t="n">
         <v>0.5415092977551711</v>
       </c>
-      <c r="D92" t="inlineStr"/>
+      <c r="D92" t="n">
+        <v>1047</v>
+      </c>
       <c r="E92" t="inlineStr">
         <is>
           <t>MSTN_059</t>
@@ -2656,7 +2838,9 @@
       <c r="C93" t="n">
         <v>1.503492665239453</v>
       </c>
-      <c r="D93" t="inlineStr"/>
+      <c r="D93" t="n">
+        <v>2960</v>
+      </c>
       <c r="E93" t="inlineStr">
         <is>
           <t>MSTN_055</t>
@@ -2680,7 +2864,9 @@
       <c r="C94" t="n">
         <v>2.712232189838863</v>
       </c>
-      <c r="D94" t="inlineStr"/>
+      <c r="D94" t="n">
+        <v>3879</v>
+      </c>
       <c r="E94" t="inlineStr">
         <is>
           <t>MSTN_046</t>
@@ -2704,7 +2890,9 @@
       <c r="C95" t="n">
         <v>4.011345202716445</v>
       </c>
-      <c r="D95" t="inlineStr"/>
+      <c r="D95" t="n">
+        <v>6176</v>
+      </c>
       <c r="E95" t="inlineStr">
         <is>
           <t>MSTN_045</t>
@@ -2728,7 +2916,9 @@
       <c r="C96" t="n">
         <v>1.226261747355102</v>
       </c>
-      <c r="D96" t="inlineStr"/>
+      <c r="D96" t="n">
+        <v>3915</v>
+      </c>
       <c r="E96" t="inlineStr">
         <is>
           <t>MSTN_091</t>
@@ -2752,7 +2942,9 @@
       <c r="C97" t="n">
         <v>5.365381132169951</v>
       </c>
-      <c r="D97" t="inlineStr"/>
+      <c r="D97" t="n">
+        <v>7549</v>
+      </c>
       <c r="E97" t="inlineStr">
         <is>
           <t>MSTN_040</t>
@@ -2776,7 +2968,9 @@
       <c r="C98" t="n">
         <v>0</v>
       </c>
-      <c r="D98" t="inlineStr"/>
+      <c r="D98" t="n">
+        <v>0</v>
+      </c>
       <c r="E98" t="inlineStr">
         <is>
           <t>MSTN_095</t>

</xml_diff>